<commit_message>
small adjustemt to assay file sample column handling
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C6C83D-356B-438E-9CA8-C0939B2A3A4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9F929C-FDF7-4486-8EA4-709E1993E9AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Source Name</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>user-specific</t>
+  </si>
+  <si>
+    <t>Sample1</t>
   </si>
 </sst>
 </file>
@@ -278,13 +281,13 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;square centimeter&quot;"/>
+      <numFmt numFmtId="164" formatCode="0.00\ &quot;degree Celsius&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00\ &quot;hour&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;square centimeter&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -304,7 +307,7 @@
   <autoFilter ref="A2:Z3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{E7EA2633-9FEF-4DBF-BE25-094306D762A3}" name="Source Name"/>
-    <tableColumn id="15" xr3:uid="{79636DF3-490C-4E3E-9F47-FCD6E480CC36}" name="Characteristics [leaf size]" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{79636DF3-490C-4E3E-9F47-FCD6E480CC36}" name="Characteristics [leaf size]" dataDxfId="4"/>
     <tableColumn id="16" xr3:uid="{BA762E53-8C3D-43DB-9924-A5594E6BA738}" name="Term Source REF [leaf size] (#h; #tTO:0002637)"/>
     <tableColumn id="17" xr3:uid="{86873A0D-C5CF-4AA8-BBCC-B67E292AF590}" name="Term Accession Number [leaf size] (#h; #tTO:0002637)"/>
     <tableColumn id="18" xr3:uid="{2889BCD1-00CB-4950-B3F1-F1FB5712FB80}" name="Unit [square centimeter] (#h; #tUO:0000081; #u)"/>
@@ -316,7 +319,7 @@
     <tableColumn id="12" xr3:uid="{6A8068B5-4279-45E4-BE6D-514641169F8A}" name="Unit [hour] (#h; #tUO:0000032; #u)"/>
     <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF [hour] (#h; #tUO:0000032; #u)"/>
     <tableColumn id="14" xr3:uid="{44FD3E41-B2D4-4AE1-A172-DB998C624864}" name="Term Accession Number [hour] (#h; #tUO:0000032; #u)"/>
-    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit]" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit]" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{13FC855C-17C7-4D8A-97EA-E441CEC0C1D6}" name="Term Source REF [temperature unit] (#h; #tUO:0000005)"/>
     <tableColumn id="5" xr3:uid="{3A277CAE-CF4C-4CE0-A152-95A430FC78F8}" name="Term Accession Number [temperature unit] (#h; #tUO:0000005)"/>
     <tableColumn id="6" xr3:uid="{34B6B618-D742-49D6-992D-F16FF943EFAB}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
@@ -617,50 +620,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="W2" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.61328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.15234375" customWidth="1"/>
-    <col min="4" max="4" width="48.4609375" customWidth="1"/>
-    <col min="5" max="5" width="43.84375" customWidth="1"/>
-    <col min="6" max="6" width="54.3828125" customWidth="1"/>
-    <col min="7" max="7" width="60.69140625" customWidth="1"/>
-    <col min="8" max="8" width="13.765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.69140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="48" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="32.3828125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="42.921875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="49.23046875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="28.15234375" customWidth="1"/>
-    <col min="15" max="15" width="50.3828125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="56.69140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="40.3828125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="50.921875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="57.23046875" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="24.84375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.4609375" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="53.765625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="53.84375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="60.15234375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="53.84375" customWidth="1"/>
-    <col min="28" max="28" width="60.15234375" customWidth="1"/>
-    <col min="29" max="29" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="52.3046875" customWidth="1"/>
-    <col min="31" max="31" width="58.53515625" customWidth="1"/>
-    <col min="32" max="32" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="52.3046875" customWidth="1"/>
-    <col min="34" max="34" width="58.53515625" customWidth="1"/>
-    <col min="35" max="35" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="42.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="49.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="15" max="15" width="50.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="56.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="40.42578125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="50.85546875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="57.28515625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.42578125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="53.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="53.85546875" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="60.140625" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="53.85546875" customWidth="1"/>
+    <col min="28" max="28" width="60.140625" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="52.28515625" customWidth="1"/>
+    <col min="31" max="31" width="58.5703125" customWidth="1"/>
+    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="52.28515625" customWidth="1"/>
+    <col min="34" max="34" width="58.5703125" customWidth="1"/>
+    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -697,7 +700,7 @@
       <c r="AH1" s="4"/>
       <c r="AI1" s="2"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -777,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -854,7 +857,7 @@
         <v>30</v>
       </c>
       <c r="Z3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tests to match assay.xlsx reader changes
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9F929C-FDF7-4486-8EA4-709E1993E9AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF916852-ABC6-4B8B-99AA-0A787B617326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Source Name</t>
   </si>
@@ -33,69 +33,12 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>Parameter [temperature unit]</t>
-  </si>
-  <si>
-    <t>Term Source REF [temperature unit] (#h; #tUO:0000005)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [temperature unit] (#h; #tUO:0000005)</t>
-  </si>
-  <si>
-    <t>Unit [degree Celsius] (#h; #tUO:0000027; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)</t>
-  </si>
-  <si>
-    <t>Factor [time]</t>
-  </si>
-  <si>
-    <t>Term Source REF [time] (#h; #tPATO:0000165)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [time] (#h; #tPATO:0000165)</t>
-  </si>
-  <si>
-    <t>Unit [hour] (#h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [hour] (#h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [hour] (#h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
     <t>Characteristics [leaf size]</t>
   </si>
   <si>
-    <t>Term Source REF [leaf size] (#h; #tTO:0002637)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [leaf size] (#h; #tTO:0002637)</t>
-  </si>
-  <si>
-    <t>Unit [square centimeter] (#h; #tUO:0000081; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [square centimeter] (#h; #tUO:0000081; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [square centimeter] (#h; #tUO:0000081; #u)</t>
-  </si>
-  <si>
     <t>Parameter [heating block]</t>
   </si>
   <si>
-    <t>Term Source REF [heating block] (#h; #tOBI:0400108)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [heating block] (#h; #tOBI:0400108)</t>
-  </si>
-  <si>
     <t>Source1</t>
   </si>
   <si>
@@ -105,12 +48,6 @@
     <t>Parameter [measurement device]</t>
   </si>
   <si>
-    <t>Term Source REF [measurement device] (#h; #tOBI:0000832)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [measurement device] (#h; #tOBI:0000832)</t>
-  </si>
-  <si>
     <t>Bruker NMR probe</t>
   </si>
   <si>
@@ -120,12 +57,6 @@
     <t>http://purl.obolibrary.org/obo/OBI_0000561</t>
   </si>
   <si>
-    <t>TO</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/TO_0002637</t>
-  </si>
-  <si>
     <t>square centimeter</t>
   </si>
   <si>
@@ -135,21 +66,12 @@
     <t>http://purl.obolibrary.org/obo/UO_0000081</t>
   </si>
   <si>
-    <t>PATO</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/PATO_0000165</t>
-  </si>
-  <si>
     <t>hour</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0000032</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000005</t>
-  </si>
-  <si>
     <t>degree Celsius</t>
   </si>
   <si>
@@ -160,6 +82,51 @@
   </si>
   <si>
     <t>Sample1</t>
+  </si>
+  <si>
+    <t>Term Source REF (TO:0002637)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (TO:0002637)</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Unit (#2)</t>
+  </si>
+  <si>
+    <t>Unit (#3)</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0400108)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0400108)</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0000832)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0000832)</t>
+  </si>
+  <si>
+    <t>Parameter [temperature unit#3]</t>
+  </si>
+  <si>
+    <t>Term Source REF (UO:0000005#3)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (UO:0000005#3)</t>
+  </si>
+  <si>
+    <t>Factor [time#2]</t>
+  </si>
+  <si>
+    <t>Term Source REF (PATO:0000165#2)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (PATO:0000165#2)</t>
   </si>
 </sst>
 </file>
@@ -303,34 +270,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC35055-8D58-440C-BAE3-31953EAFEC50}" name="annotationTable" displayName="annotationTable" ref="A2:Z3" totalsRowShown="0">
-  <autoFilter ref="A2:Z3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC35055-8D58-440C-BAE3-31953EAFEC50}" name="annotationTable" displayName="annotationTable" ref="A2:T3" totalsRowShown="0">
+  <autoFilter ref="A2:T3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{E7EA2633-9FEF-4DBF-BE25-094306D762A3}" name="Source Name"/>
     <tableColumn id="15" xr3:uid="{79636DF3-490C-4E3E-9F47-FCD6E480CC36}" name="Characteristics [leaf size]" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{BA762E53-8C3D-43DB-9924-A5594E6BA738}" name="Term Source REF [leaf size] (#h; #tTO:0002637)"/>
-    <tableColumn id="17" xr3:uid="{86873A0D-C5CF-4AA8-BBCC-B67E292AF590}" name="Term Accession Number [leaf size] (#h; #tTO:0002637)"/>
-    <tableColumn id="18" xr3:uid="{2889BCD1-00CB-4950-B3F1-F1FB5712FB80}" name="Unit [square centimeter] (#h; #tUO:0000081; #u)"/>
-    <tableColumn id="19" xr3:uid="{CC1A8923-671C-4315-84D1-7AAC29CEC702}" name="Term Source REF [square centimeter] (#h; #tUO:0000081; #u)"/>
-    <tableColumn id="20" xr3:uid="{948D772D-CCB9-47D9-9C1B-6FFFAA63A7F6}" name="Term Accession Number [square centimeter] (#h; #tUO:0000081; #u)" dataCellStyle="Hyperlink"/>
-    <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time]" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{9A99257D-18F4-415D-88A2-593C91006B72}" name="Term Source REF [time] (#h; #tPATO:0000165)"/>
-    <tableColumn id="11" xr3:uid="{103A9A8B-FF32-4462-9E05-3E659FE49841}" name="Term Accession Number [time] (#h; #tPATO:0000165)"/>
-    <tableColumn id="12" xr3:uid="{6A8068B5-4279-45E4-BE6D-514641169F8A}" name="Unit [hour] (#h; #tUO:0000032; #u)"/>
-    <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF [hour] (#h; #tUO:0000032; #u)"/>
-    <tableColumn id="14" xr3:uid="{44FD3E41-B2D4-4AE1-A172-DB998C624864}" name="Term Accession Number [hour] (#h; #tUO:0000032; #u)"/>
-    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit]" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{13FC855C-17C7-4D8A-97EA-E441CEC0C1D6}" name="Term Source REF [temperature unit] (#h; #tUO:0000005)"/>
-    <tableColumn id="5" xr3:uid="{3A277CAE-CF4C-4CE0-A152-95A430FC78F8}" name="Term Accession Number [temperature unit] (#h; #tUO:0000005)"/>
-    <tableColumn id="6" xr3:uid="{34B6B618-D742-49D6-992D-F16FF943EFAB}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="7" xr3:uid="{5B634ABC-9CAF-49DD-870C-E1BB8914A053}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="8" xr3:uid="{2B65DE09-5B77-4672-BA62-DF26E7005B9F}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)"/>
+    <tableColumn id="18" xr3:uid="{2889BCD1-00CB-4950-B3F1-F1FB5712FB80}" name="Unit"/>
+    <tableColumn id="19" xr3:uid="{CC1A8923-671C-4315-84D1-7AAC29CEC702}" name="Term Source REF (TO:0002637)"/>
+    <tableColumn id="20" xr3:uid="{948D772D-CCB9-47D9-9C1B-6FFFAA63A7F6}" name="Term Accession Number (TO:0002637)" dataCellStyle="Hyperlink"/>
+    <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time#2]" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{6A8068B5-4279-45E4-BE6D-514641169F8A}" name="Unit (#2)"/>
+    <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF (PATO:0000165#2)"/>
+    <tableColumn id="14" xr3:uid="{44FD3E41-B2D4-4AE1-A172-DB998C624864}" name="Term Accession Number (PATO:0000165#2)"/>
+    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit#3]" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{34B6B618-D742-49D6-992D-F16FF943EFAB}" name="Unit (#3)"/>
+    <tableColumn id="7" xr3:uid="{5B634ABC-9CAF-49DD-870C-E1BB8914A053}" name="Term Source REF (UO:0000005#3)"/>
+    <tableColumn id="8" xr3:uid="{2B65DE09-5B77-4672-BA62-DF26E7005B9F}" name="Term Accession Number (UO:0000005#3)"/>
     <tableColumn id="24" xr3:uid="{C28C70F4-0883-474E-ABCB-81751DE2164F}" name="Parameter [heating block]" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{F7F11425-7F02-413B-84ED-3BA40C8A0605}" name="Term Source REF [heating block] (#h; #tOBI:0400108)"/>
-    <tableColumn id="26" xr3:uid="{B6497CE0-7B53-4356-832B-EA8E0B30DFB1}" name="Term Accession Number [heating block] (#h; #tOBI:0400108)"/>
+    <tableColumn id="25" xr3:uid="{F7F11425-7F02-413B-84ED-3BA40C8A0605}" name="Term Source REF (OBI:0400108)"/>
+    <tableColumn id="26" xr3:uid="{B6497CE0-7B53-4356-832B-EA8E0B30DFB1}" name="Term Accession Number (OBI:0400108)"/>
     <tableColumn id="36" xr3:uid="{4A03BD7B-9C02-4AD0-8AAA-835B77C05627}" name="Parameter [measurement device]" dataDxfId="0"/>
-    <tableColumn id="37" xr3:uid="{F2577B7A-2690-4225-9F9E-82A829C82796}" name="Term Source REF [measurement device] (#h; #tOBI:0000832)"/>
-    <tableColumn id="38" xr3:uid="{EC488F0F-3CE1-4706-AA24-31F894E35837}" name="Term Accession Number [measurement device] (#h; #tOBI:0000832)"/>
+    <tableColumn id="37" xr3:uid="{F2577B7A-2690-4225-9F9E-82A829C82796}" name="Term Source REF (OBI:0000832)"/>
+    <tableColumn id="38" xr3:uid="{EC488F0F-3CE1-4706-AA24-31F894E35837}" name="Term Accession Number (OBI:0000832)"/>
     <tableColumn id="2" xr3:uid="{B5E6C947-CECD-4B52-A414-DAA66A89B993}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -618,52 +579,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W2" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" customWidth="1"/>
-    <col min="7" max="7" width="60.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="48" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="42.85546875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="49.28515625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="15" max="15" width="50.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="40.42578125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="50.85546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="57.28515625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.42578125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="53.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="53.85546875" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="60.140625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="53.85546875" customWidth="1"/>
-    <col min="28" max="28" width="60.140625" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="52.28515625" customWidth="1"/>
-    <col min="31" max="31" width="58.5703125" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="52.28515625" customWidth="1"/>
-    <col min="34" max="34" width="58.5703125" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.84375" customWidth="1"/>
+    <col min="4" max="4" width="54.3828125" customWidth="1"/>
+    <col min="5" max="5" width="60.69140625" customWidth="1"/>
+    <col min="6" max="6" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.3828125" customWidth="1"/>
+    <col min="8" max="8" width="42.84375" customWidth="1"/>
+    <col min="9" max="9" width="49.3046875" customWidth="1"/>
+    <col min="10" max="10" width="28.15234375" customWidth="1"/>
+    <col min="11" max="11" width="40.3828125" customWidth="1"/>
+    <col min="12" max="12" width="50.84375" customWidth="1"/>
+    <col min="13" max="13" width="57.3046875" customWidth="1"/>
+    <col min="14" max="14" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.3828125" customWidth="1"/>
+    <col min="16" max="16" width="53.69140625" customWidth="1"/>
+    <col min="17" max="17" width="31.15234375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="53.84375" customWidth="1"/>
+    <col min="19" max="19" width="60.15234375" customWidth="1"/>
+    <col min="20" max="20" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="53.84375" customWidth="1"/>
+    <col min="22" max="22" width="60.15234375" customWidth="1"/>
+    <col min="23" max="23" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="52.3046875" customWidth="1"/>
+    <col min="25" max="25" width="58.53515625" customWidth="1"/>
+    <col min="26" max="26" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="52.3046875" customWidth="1"/>
+    <col min="28" max="28" width="58.53515625" customWidth="1"/>
+    <col min="29" max="29" width="14.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -692,181 +647,140 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2" t="s">
-        <v>22</v>
-      </c>
-      <c r="W2" t="s">
-        <v>25</v>
-      </c>
-      <c r="X2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
       </c>
       <c r="B3" s="6">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="5">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5">
         <v>5</v>
       </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
+        <v>14</v>
+      </c>
+      <c r="J3" s="3">
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="3">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="P3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="S3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" t="s">
-        <v>43</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="X3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>44</v>
+        <v>9</v>
+      </c>
+      <c r="T3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{A9013C06-E037-448D-836C-23E661F5FEEA}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{A9013C06-E037-448D-836C-23E661F5FEEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
small adjustment to assay.xlsx reader
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF916852-ABC6-4B8B-99AA-0A787B617326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D2ABDC-EA50-45E2-B44A-894CBB07996B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,22 +111,22 @@
     <t>Term Accession Number (OBI:0000832)</t>
   </si>
   <si>
-    <t>Parameter [temperature unit#3]</t>
-  </si>
-  <si>
-    <t>Term Source REF (UO:0000005#3)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (UO:0000005#3)</t>
-  </si>
-  <si>
-    <t>Factor [time#2]</t>
-  </si>
-  <si>
-    <t>Term Source REF (PATO:0000165#2)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (PATO:0000165#2)</t>
+    <t>Factor [time]</t>
+  </si>
+  <si>
+    <t>Term Source REF (PATO:0000165)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (PATO:0000165)</t>
+  </si>
+  <si>
+    <t>Parameter [temperature unit]</t>
+  </si>
+  <si>
+    <t>Term Source REF (UO:0000005)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (UO:0000005)</t>
   </si>
 </sst>
 </file>
@@ -278,14 +278,14 @@
     <tableColumn id="18" xr3:uid="{2889BCD1-00CB-4950-B3F1-F1FB5712FB80}" name="Unit"/>
     <tableColumn id="19" xr3:uid="{CC1A8923-671C-4315-84D1-7AAC29CEC702}" name="Term Source REF (TO:0002637)"/>
     <tableColumn id="20" xr3:uid="{948D772D-CCB9-47D9-9C1B-6FFFAA63A7F6}" name="Term Accession Number (TO:0002637)" dataCellStyle="Hyperlink"/>
-    <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time#2]" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time]" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{6A8068B5-4279-45E4-BE6D-514641169F8A}" name="Unit (#2)"/>
-    <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF (PATO:0000165#2)"/>
-    <tableColumn id="14" xr3:uid="{44FD3E41-B2D4-4AE1-A172-DB998C624864}" name="Term Accession Number (PATO:0000165#2)"/>
-    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit#3]" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF (PATO:0000165)"/>
+    <tableColumn id="14" xr3:uid="{44FD3E41-B2D4-4AE1-A172-DB998C624864}" name="Term Accession Number (PATO:0000165)"/>
+    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit]" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{34B6B618-D742-49D6-992D-F16FF943EFAB}" name="Unit (#3)"/>
-    <tableColumn id="7" xr3:uid="{5B634ABC-9CAF-49DD-870C-E1BB8914A053}" name="Term Source REF (UO:0000005#3)"/>
-    <tableColumn id="8" xr3:uid="{2B65DE09-5B77-4672-BA62-DF26E7005B9F}" name="Term Accession Number (UO:0000005#3)"/>
+    <tableColumn id="7" xr3:uid="{5B634ABC-9CAF-49DD-870C-E1BB8914A053}" name="Term Source REF (UO:0000005)"/>
+    <tableColumn id="8" xr3:uid="{2B65DE09-5B77-4672-BA62-DF26E7005B9F}" name="Term Accession Number (UO:0000005)"/>
     <tableColumn id="24" xr3:uid="{C28C70F4-0883-474E-ABCB-81751DE2164F}" name="Parameter [heating block]" dataDxfId="1"/>
     <tableColumn id="25" xr3:uid="{F7F11425-7F02-413B-84ED-3BA40C8A0605}" name="Term Source REF (OBI:0400108)"/>
     <tableColumn id="26" xr3:uid="{B6497CE0-7B53-4356-832B-EA8E0B30DFB1}" name="Term Accession Number (OBI:0400108)"/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -666,28 +666,28 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
add component and protocol type reader tests
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D2ABDC-EA50-45E2-B44A-894CBB07996B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752C2955-D3F3-4341-9AA6-10E3D6C5855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Source Name</t>
   </si>
@@ -127,16 +127,71 @@
   </si>
   <si>
     <t>Term Accession Number (UO:0000005)</t>
+  </si>
+  <si>
+    <t>Term Source REF (MS:1000031)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (MS:1000031)</t>
+  </si>
+  <si>
+    <t>Orbitrap Fusion</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1002416</t>
+  </si>
+  <si>
+    <t>Unit (#4)</t>
+  </si>
+  <si>
+    <t>Term Source REF (PATO:0000128)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (PATO:0000128)</t>
+  </si>
+  <si>
+    <t>gram</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000021</t>
+  </si>
+  <si>
+    <t>Component [weight]</t>
+  </si>
+  <si>
+    <t>Component [instrument model]</t>
+  </si>
+  <si>
+    <t>Growth Protocol</t>
+  </si>
+  <si>
+    <t>NFDI4PSO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1002416</t>
+  </si>
+  <si>
+    <t>Protocol Type</t>
+  </si>
+  <si>
+    <t>Term Source REF</t>
+  </si>
+  <si>
+    <t>Term Accession Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;degree Celsius&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;hour&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;square centimeter&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;gram&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -219,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,12 +290,25 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;gram&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;gram&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;gram&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;gram&quot;"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -270,28 +338,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC35055-8D58-440C-BAE3-31953EAFEC50}" name="annotationTable" displayName="annotationTable" ref="A2:T3" totalsRowShown="0">
-  <autoFilter ref="A2:T3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC35055-8D58-440C-BAE3-31953EAFEC50}" name="annotationTable" displayName="annotationTable" ref="A2:AD3" totalsRowShown="0">
+  <autoFilter ref="A2:AD3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
+  <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{E7EA2633-9FEF-4DBF-BE25-094306D762A3}" name="Source Name"/>
-    <tableColumn id="15" xr3:uid="{79636DF3-490C-4E3E-9F47-FCD6E480CC36}" name="Characteristics [leaf size]" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{48CBC16A-F60D-4A7A-93E8-2E8F41B1D655}" name="Protocol Type"/>
+    <tableColumn id="10" xr3:uid="{F89195A1-219E-42CB-A48D-973B358A5598}" name="Term Source REF"/>
+    <tableColumn id="5" xr3:uid="{F7894637-F01B-4003-9F88-154FD3FFAA76}" name="Term Accession Number" dataCellStyle="Hyperlink"/>
+    <tableColumn id="15" xr3:uid="{79636DF3-490C-4E3E-9F47-FCD6E480CC36}" name="Characteristics [leaf size]" dataDxfId="8"/>
     <tableColumn id="18" xr3:uid="{2889BCD1-00CB-4950-B3F1-F1FB5712FB80}" name="Unit"/>
     <tableColumn id="19" xr3:uid="{CC1A8923-671C-4315-84D1-7AAC29CEC702}" name="Term Source REF (TO:0002637)"/>
     <tableColumn id="20" xr3:uid="{948D772D-CCB9-47D9-9C1B-6FFFAA63A7F6}" name="Term Accession Number (TO:0002637)" dataCellStyle="Hyperlink"/>
-    <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time]" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time]" dataDxfId="7"/>
     <tableColumn id="12" xr3:uid="{6A8068B5-4279-45E4-BE6D-514641169F8A}" name="Unit (#2)"/>
     <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF (PATO:0000165)"/>
     <tableColumn id="14" xr3:uid="{44FD3E41-B2D4-4AE1-A172-DB998C624864}" name="Term Accession Number (PATO:0000165)"/>
-    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit]" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{23085535-1F06-4217-8B0C-CC8E354AC2EC}" name="Parameter [temperature unit]" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{34B6B618-D742-49D6-992D-F16FF943EFAB}" name="Unit (#3)"/>
     <tableColumn id="7" xr3:uid="{5B634ABC-9CAF-49DD-870C-E1BB8914A053}" name="Term Source REF (UO:0000005)"/>
     <tableColumn id="8" xr3:uid="{2B65DE09-5B77-4672-BA62-DF26E7005B9F}" name="Term Accession Number (UO:0000005)"/>
-    <tableColumn id="24" xr3:uid="{C28C70F4-0883-474E-ABCB-81751DE2164F}" name="Parameter [heating block]" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{C28C70F4-0883-474E-ABCB-81751DE2164F}" name="Parameter [heating block]" dataDxfId="5"/>
     <tableColumn id="25" xr3:uid="{F7F11425-7F02-413B-84ED-3BA40C8A0605}" name="Term Source REF (OBI:0400108)"/>
     <tableColumn id="26" xr3:uid="{B6497CE0-7B53-4356-832B-EA8E0B30DFB1}" name="Term Accession Number (OBI:0400108)"/>
-    <tableColumn id="36" xr3:uid="{4A03BD7B-9C02-4AD0-8AAA-835B77C05627}" name="Parameter [measurement device]" dataDxfId="0"/>
+    <tableColumn id="36" xr3:uid="{4A03BD7B-9C02-4AD0-8AAA-835B77C05627}" name="Parameter [measurement device]" dataDxfId="4"/>
     <tableColumn id="37" xr3:uid="{F2577B7A-2690-4225-9F9E-82A829C82796}" name="Term Source REF (OBI:0000832)"/>
     <tableColumn id="38" xr3:uid="{EC488F0F-3CE1-4706-AA24-31F894E35837}" name="Term Accession Number (OBI:0000832)"/>
+    <tableColumn id="11" xr3:uid="{9F1607B2-9FC5-4AD5-9177-35C142DD60C4}" name="Component [instrument model]"/>
+    <tableColumn id="16" xr3:uid="{440641B4-85D6-40F4-80E1-26F77E15C3B6}" name="Term Source REF (MS:1000031)"/>
+    <tableColumn id="17" xr3:uid="{4129639C-F19F-4F93-AD36-D57C12690A4C}" name="Term Accession Number (MS:1000031)" dataCellStyle="Hyperlink"/>
+    <tableColumn id="28" xr3:uid="{82AC190F-A789-4E21-B7A8-B70226F9602A}" name="Component [weight]" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{D58D63AB-C7D9-4C19-90D2-6A7AA339661A}" name="Unit (#4)" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{0C87C796-7D2A-4BD9-A488-FDB632C9C546}" name="Term Source REF (PATO:0000128)" dataDxfId="1"/>
+    <tableColumn id="31" xr3:uid="{75FD7A16-C0F0-4D2E-B2CC-070DE44688F0}" name="Term Accession Number (PATO:0000128)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{B5E6C947-CECD-4B52-A414-DAA66A89B993}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -561,7 +639,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="1217" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="613" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -579,50 +657,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.84375" customWidth="1"/>
-    <col min="4" max="4" width="54.3828125" customWidth="1"/>
-    <col min="5" max="5" width="60.69140625" customWidth="1"/>
-    <col min="6" max="6" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.3828125" customWidth="1"/>
-    <col min="8" max="8" width="42.84375" customWidth="1"/>
-    <col min="9" max="9" width="49.3046875" customWidth="1"/>
-    <col min="10" max="10" width="28.15234375" customWidth="1"/>
-    <col min="11" max="11" width="40.3828125" customWidth="1"/>
-    <col min="12" max="12" width="50.84375" customWidth="1"/>
-    <col min="13" max="13" width="57.3046875" customWidth="1"/>
-    <col min="14" max="14" width="24.84375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="47.3828125" customWidth="1"/>
-    <col min="16" max="16" width="53.69140625" customWidth="1"/>
-    <col min="17" max="17" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="53.84375" customWidth="1"/>
-    <col min="19" max="19" width="60.15234375" customWidth="1"/>
-    <col min="20" max="20" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="53.84375" customWidth="1"/>
-    <col min="22" max="22" width="60.15234375" customWidth="1"/>
-    <col min="23" max="23" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="52.3046875" customWidth="1"/>
-    <col min="25" max="25" width="58.53515625" customWidth="1"/>
-    <col min="26" max="26" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="52.3046875" customWidth="1"/>
-    <col min="28" max="28" width="58.53515625" customWidth="1"/>
-    <col min="29" max="29" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.07421875" customWidth="1"/>
+    <col min="5" max="5" width="23.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.84375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="54.3828125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="60.69140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.3828125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.84375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="49.3046875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="28.15234375" customWidth="1"/>
+    <col min="14" max="14" width="40.3828125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="50.84375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="57.3046875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47.3828125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="53.69140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="31.15234375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.3828125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="12.4609375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="27.84375" customWidth="1"/>
+    <col min="24" max="24" width="16" customWidth="1"/>
+    <col min="25" max="25" width="51.07421875" customWidth="1"/>
+    <col min="26" max="26" width="19.3046875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.765625" customWidth="1"/>
+    <col min="28" max="28" width="40.4609375" customWidth="1"/>
+    <col min="29" max="29" width="41.15234375" customWidth="1"/>
+    <col min="30" max="30" width="14.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -647,140 +724,203 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
-      <c r="AC1" s="2"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>24</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>6</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>26</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>27</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="6">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5">
+      <c r="I3" s="5">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="3">
+      <c r="M3" s="3">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>11</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>8</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>9</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{A9013C06-E037-448D-836C-23E661F5FEEA}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{A9013C06-E037-448D-836C-23E661F5FEEA}"/>
+    <hyperlink ref="Y3" r:id="rId2" xr:uid="{FFEE82C9-A55A-4C62-84B0-C9A66A93291A}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{E92F0F06-7C60-4547-B31C-2E15D1D8116B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add protocol ref parsing test
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752C2955-D3F3-4341-9AA6-10E3D6C5855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C262A845-971A-48E9-9A52-565C1776C1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Source Name</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>Term Accession Number</t>
+  </si>
+  <si>
+    <t>Protocol REF</t>
+  </si>
+  <si>
+    <t>MyProtocol</t>
   </si>
 </sst>
 </file>
@@ -338,10 +344,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC35055-8D58-440C-BAE3-31953EAFEC50}" name="annotationTable" displayName="annotationTable" ref="A2:AD3" totalsRowShown="0">
-  <autoFilter ref="A2:AD3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
-  <tableColumns count="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC35055-8D58-440C-BAE3-31953EAFEC50}" name="annotationTable" displayName="annotationTable" ref="A2:AE3" totalsRowShown="0">
+  <autoFilter ref="A2:AE3" xr:uid="{40B0238E-DE7B-4500-9DF5-19BC08DE089A}"/>
+  <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{E7EA2633-9FEF-4DBF-BE25-094306D762A3}" name="Source Name"/>
+    <tableColumn id="4" xr3:uid="{5873DA80-A332-4C38-B7BE-A7004C655F19}" name="Protocol REF"/>
     <tableColumn id="21" xr3:uid="{48CBC16A-F60D-4A7A-93E8-2E8F41B1D655}" name="Protocol Type"/>
     <tableColumn id="10" xr3:uid="{F89195A1-219E-42CB-A48D-973B358A5598}" name="Term Source REF"/>
     <tableColumn id="5" xr3:uid="{F7894637-F01B-4003-9F88-154FD3FFAA76}" name="Term Accession Number" dataCellStyle="Hyperlink"/>
@@ -657,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -695,7 +702,7 @@
     <col min="30" max="30" width="14.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -727,195 +734,201 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>31</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>3</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>24</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>25</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>6</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>27</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>45</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>44</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="5">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>27</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>11</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="R3" t="s">
-        <v>17</v>
       </c>
       <c r="S3" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>8</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>9</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>36</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Z3" s="9">
+      <c r="AA3" s="9">
         <v>12</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AB3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AC3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AD3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{A9013C06-E037-448D-836C-23E661F5FEEA}"/>
-    <hyperlink ref="Y3" r:id="rId2" xr:uid="{FFEE82C9-A55A-4C62-84B0-C9A66A93291A}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{E92F0F06-7C60-4547-B31C-2E15D1D8116B}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{A9013C06-E037-448D-836C-23E661F5FEEA}"/>
+    <hyperlink ref="Z3" r:id="rId2" xr:uid="{FFEE82C9-A55A-4C62-84B0-C9A66A93291A}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{E92F0F06-7C60-4547-B31C-2E15D1D8116B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
update assay xlsx reader tests for Swate 0.7.0 compatability
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTableTestFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C262A845-971A-48E9-9A52-565C1776C1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87159A07-BAAA-4EF6-BE85-0B5234016591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>http://purl.obolibrary.org/obo/MS_1002416</t>
   </si>
   <si>
-    <t>Unit (#4)</t>
-  </si>
-  <si>
     <t>Term Source REF (PATO:0000128)</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>MyProtocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit   </t>
   </si>
 </sst>
 </file>
@@ -299,8 +299,8 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -351,11 +351,11 @@
     <tableColumn id="4" xr3:uid="{5873DA80-A332-4C38-B7BE-A7004C655F19}" name="Protocol REF"/>
     <tableColumn id="21" xr3:uid="{48CBC16A-F60D-4A7A-93E8-2E8F41B1D655}" name="Protocol Type"/>
     <tableColumn id="10" xr3:uid="{F89195A1-219E-42CB-A48D-973B358A5598}" name="Term Source REF"/>
-    <tableColumn id="5" xr3:uid="{F7894637-F01B-4003-9F88-154FD3FFAA76}" name="Term Accession Number" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{F7894637-F01B-4003-9F88-154FD3FFAA76}" name="Term Accession Number"/>
     <tableColumn id="15" xr3:uid="{79636DF3-490C-4E3E-9F47-FCD6E480CC36}" name="Characteristics [leaf size]" dataDxfId="8"/>
     <tableColumn id="18" xr3:uid="{2889BCD1-00CB-4950-B3F1-F1FB5712FB80}" name="Unit"/>
     <tableColumn id="19" xr3:uid="{CC1A8923-671C-4315-84D1-7AAC29CEC702}" name="Term Source REF (TO:0002637)"/>
-    <tableColumn id="20" xr3:uid="{948D772D-CCB9-47D9-9C1B-6FFFAA63A7F6}" name="Term Accession Number (TO:0002637)" dataCellStyle="Hyperlink"/>
+    <tableColumn id="20" xr3:uid="{948D772D-CCB9-47D9-9C1B-6FFFAA63A7F6}" name="Term Accession Number (TO:0002637)"/>
     <tableColumn id="9" xr3:uid="{D15A1001-9EE5-4759-8B83-0D2108C2D88E}" name="Factor [time]" dataDxfId="7"/>
     <tableColumn id="12" xr3:uid="{6A8068B5-4279-45E4-BE6D-514641169F8A}" name="Unit (#2)"/>
     <tableColumn id="13" xr3:uid="{79B0E4B9-E915-4B6C-AD0B-E41477C56DB7}" name="Term Source REF (PATO:0000165)"/>
@@ -372,9 +372,9 @@
     <tableColumn id="38" xr3:uid="{EC488F0F-3CE1-4706-AA24-31F894E35837}" name="Term Accession Number (OBI:0000832)"/>
     <tableColumn id="11" xr3:uid="{9F1607B2-9FC5-4AD5-9177-35C142DD60C4}" name="Component [instrument model]"/>
     <tableColumn id="16" xr3:uid="{440641B4-85D6-40F4-80E1-26F77E15C3B6}" name="Term Source REF (MS:1000031)"/>
-    <tableColumn id="17" xr3:uid="{4129639C-F19F-4F93-AD36-D57C12690A4C}" name="Term Accession Number (MS:1000031)" dataCellStyle="Hyperlink"/>
+    <tableColumn id="17" xr3:uid="{4129639C-F19F-4F93-AD36-D57C12690A4C}" name="Term Accession Number (MS:1000031)"/>
     <tableColumn id="28" xr3:uid="{82AC190F-A789-4E21-B7A8-B70226F9602A}" name="Component [weight]" dataDxfId="3"/>
-    <tableColumn id="29" xr3:uid="{D58D63AB-C7D9-4C19-90D2-6A7AA339661A}" name="Unit (#4)" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{D58D63AB-C7D9-4C19-90D2-6A7AA339661A}" name="Unit   " dataDxfId="2"/>
     <tableColumn id="30" xr3:uid="{0C87C796-7D2A-4BD9-A488-FDB632C9C546}" name="Term Source REF (PATO:0000128)" dataDxfId="1"/>
     <tableColumn id="31" xr3:uid="{75FD7A16-C0F0-4D2E-B2CC-070DE44688F0}" name="Term Accession Number (PATO:0000128)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{B5E6C947-CECD-4B52-A414-DAA66A89B993}" name="Sample Name"/>
@@ -666,43 +666,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.07421875" customWidth="1"/>
-    <col min="5" max="5" width="23.61328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.84375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="54.3828125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="60.69140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.3828125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="42.84375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="49.3046875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="28.15234375" customWidth="1"/>
-    <col min="14" max="14" width="40.3828125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="50.84375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="57.3046875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="24.84375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="47.3828125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="53.69140625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.3828125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.4609375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="27.84375" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.81640625" customWidth="1"/>
+    <col min="7" max="7" width="54.36328125" customWidth="1"/>
+    <col min="8" max="8" width="60.7265625" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.36328125" customWidth="1"/>
+    <col min="11" max="11" width="42.81640625" customWidth="1"/>
+    <col min="12" max="12" width="49.26953125" customWidth="1"/>
+    <col min="13" max="13" width="28.1796875" customWidth="1"/>
+    <col min="14" max="14" width="40.36328125" customWidth="1"/>
+    <col min="15" max="15" width="50.81640625" customWidth="1"/>
+    <col min="16" max="16" width="57.26953125" customWidth="1"/>
+    <col min="17" max="17" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47.36328125" customWidth="1"/>
+    <col min="19" max="19" width="53.7265625" customWidth="1"/>
+    <col min="20" max="20" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.36328125" customWidth="1"/>
+    <col min="22" max="22" width="12.453125" customWidth="1"/>
+    <col min="23" max="23" width="27.81640625" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="51.07421875" customWidth="1"/>
-    <col min="26" max="26" width="19.3046875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.765625" customWidth="1"/>
-    <col min="28" max="28" width="40.4609375" customWidth="1"/>
-    <col min="29" max="29" width="41.15234375" customWidth="1"/>
-    <col min="30" max="30" width="14.61328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="51.08984375" customWidth="1"/>
+    <col min="26" max="26" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.7265625" customWidth="1"/>
+    <col min="28" max="28" width="40.453125" customWidth="1"/>
+    <col min="29" max="29" width="41.1796875" customWidth="1"/>
+    <col min="30" max="30" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -734,21 +734,21 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -805,7 +805,7 @@
         <v>27</v>
       </c>
       <c r="X2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y2" t="s">
         <v>34</v>
@@ -814,36 +814,36 @@
         <v>35</v>
       </c>
       <c r="AA2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>40</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>41</v>
       </c>
       <c r="AE2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="F3" s="6">
         <v>10</v>
@@ -912,13 +912,13 @@
         <v>12</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AC3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="AD3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE3" t="s">
         <v>18</v>

</xml_diff>